<commit_message>
added region/disclaimer in notebook for openpyxl | Concluded that rebuild function is completed for the purpose (require strike-thru texts to also be colored for 100% functionality).
</commit_message>
<xml_diff>
--- a/sample_data/output_test.xlsx
+++ b/sample_data/output_test.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <bookViews>
-    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
+    <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" xWindow="-93" yWindow="-93" windowWidth="23226" windowHeight="14586" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
     <sheet name="737MAX EDFCS Requirements_Valid" sheetId="1" state="visible" r:id="rId1"/>
@@ -16,7 +16,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <numFmts count="0"/>
-  <fonts count="25">
+  <fonts count="26">
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -200,6 +200,13 @@
     <font>
       <name val="Aptos Narrow"/>
       <family val="2"/>
+      <sz val="11"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <strike val="1"/>
       <sz val="11"/>
       <scheme val="minor"/>
     </font>
@@ -572,7 +579,7 @@
     <xf numFmtId="0" fontId="1" fillId="31" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="32" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="34" borderId="10" pivotButton="0" quotePrefix="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
@@ -591,10 +598,7 @@
     <xf numFmtId="0" fontId="21" fillId="0" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="33" borderId="10" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
-      <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="24" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" applyAlignment="1" pivotButton="0" quotePrefix="0" xfId="0">
       <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -972,56 +976,56 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="8" defaultColWidth="9.1171875" defaultRowHeight="14.35"/>
   <cols>
-    <col width="24.140625" customWidth="1" style="5" min="1" max="1"/>
-    <col width="32.140625" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
+    <col width="24.1171875" customWidth="1" style="5" min="1" max="1"/>
+    <col width="32.1171875" bestFit="1" customWidth="1" style="5" min="2" max="2"/>
     <col width="37" customWidth="1" style="5" min="3" max="3"/>
-    <col width="29.42578125" customWidth="1" style="5" min="4" max="4"/>
-    <col width="25.5703125" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
-    <col width="29.42578125" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
-    <col width="7.5703125" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
-    <col width="17.42578125" bestFit="1" customWidth="1" style="5" min="8" max="8"/>
-    <col width="21.85546875" bestFit="1" customWidth="1" style="5" min="9" max="9"/>
-    <col width="20.28515625" bestFit="1" customWidth="1" style="5" min="10" max="10"/>
-    <col width="22.140625" bestFit="1" customWidth="1" style="5" min="11" max="11"/>
-    <col width="31.5703125" bestFit="1" customWidth="1" style="5" min="12" max="12"/>
-    <col width="13.140625" bestFit="1" customWidth="1" style="5" min="13" max="13"/>
-    <col width="6.140625" bestFit="1" customWidth="1" style="5" min="14" max="14"/>
+    <col width="29.41015625" customWidth="1" style="5" min="4" max="4"/>
+    <col width="25.5859375" bestFit="1" customWidth="1" style="5" min="5" max="5"/>
+    <col width="29.41015625" bestFit="1" customWidth="1" style="5" min="6" max="6"/>
+    <col width="7.5859375" bestFit="1" customWidth="1" style="5" min="7" max="7"/>
+    <col width="17.41015625" bestFit="1" customWidth="1" style="5" min="8" max="8"/>
+    <col width="21.87890625" bestFit="1" customWidth="1" style="5" min="9" max="9"/>
+    <col width="20.29296875" bestFit="1" customWidth="1" style="5" min="10" max="10"/>
+    <col width="22.1171875" bestFit="1" customWidth="1" style="5" min="11" max="11"/>
+    <col width="31.5859375" bestFit="1" customWidth="1" style="5" min="12" max="12"/>
+    <col width="13.1171875" bestFit="1" customWidth="1" style="5" min="13" max="13"/>
+    <col width="6.1171875" bestFit="1" customWidth="1" style="5" min="14" max="14"/>
     <col width="23" bestFit="1" customWidth="1" style="5" min="15" max="15"/>
-    <col width="6.7109375" bestFit="1" customWidth="1" style="5" min="16" max="16"/>
+    <col width="6.703125" bestFit="1" customWidth="1" style="5" min="16" max="16"/>
     <col width="14" bestFit="1" customWidth="1" style="5" min="17" max="17"/>
-    <col width="13.42578125" bestFit="1" customWidth="1" style="5" min="18" max="18"/>
+    <col width="13.41015625" bestFit="1" customWidth="1" style="5" min="18" max="18"/>
     <col width="11" bestFit="1" customWidth="1" style="5" min="19" max="19"/>
-    <col width="25.140625" bestFit="1" customWidth="1" style="5" min="20" max="20"/>
-    <col width="28.28515625" bestFit="1" customWidth="1" style="5" min="21" max="21"/>
+    <col width="25.1171875" bestFit="1" customWidth="1" style="5" min="20" max="20"/>
+    <col width="28.29296875" bestFit="1" customWidth="1" style="5" min="21" max="21"/>
     <col width="29" bestFit="1" customWidth="1" style="5" min="22" max="22"/>
-    <col width="28.42578125" bestFit="1" customWidth="1" style="5" min="23" max="23"/>
+    <col width="28.41015625" bestFit="1" customWidth="1" style="5" min="23" max="23"/>
     <col width="29" bestFit="1" customWidth="1" style="5" min="24" max="24"/>
-    <col width="19.7109375" bestFit="1" customWidth="1" style="5" min="25" max="25"/>
-    <col width="41.28515625" bestFit="1" customWidth="1" style="5" min="26" max="26"/>
-    <col width="32.5703125" bestFit="1" customWidth="1" style="5" min="27" max="27"/>
-    <col width="30.85546875" bestFit="1" customWidth="1" style="5" min="28" max="28"/>
-    <col width="36.140625" bestFit="1" customWidth="1" style="5" min="29" max="29"/>
-    <col width="49.5703125" bestFit="1" customWidth="1" style="5" min="30" max="30"/>
-    <col width="16.140625" bestFit="1" customWidth="1" style="5" min="31" max="31"/>
-    <col width="17.42578125" bestFit="1" customWidth="1" style="5" min="32" max="32"/>
-    <col width="18.5703125" bestFit="1" customWidth="1" style="5" min="33" max="33"/>
-    <col width="33.140625" bestFit="1" customWidth="1" style="5" min="34" max="34"/>
-    <col width="56.5703125" bestFit="1" customWidth="1" style="5" min="35" max="35"/>
-    <col width="33.140625" bestFit="1" customWidth="1" style="5" min="36" max="36"/>
+    <col width="19.703125" bestFit="1" customWidth="1" style="5" min="25" max="25"/>
+    <col width="41.29296875" bestFit="1" customWidth="1" style="5" min="26" max="26"/>
+    <col width="32.5859375" bestFit="1" customWidth="1" style="5" min="27" max="27"/>
+    <col width="30.87890625" bestFit="1" customWidth="1" style="5" min="28" max="28"/>
+    <col width="36.1171875" bestFit="1" customWidth="1" style="5" min="29" max="29"/>
+    <col width="49.5859375" bestFit="1" customWidth="1" style="5" min="30" max="30"/>
+    <col width="16.1171875" bestFit="1" customWidth="1" style="5" min="31" max="31"/>
+    <col width="17.41015625" bestFit="1" customWidth="1" style="5" min="32" max="32"/>
+    <col width="18.5859375" bestFit="1" customWidth="1" style="5" min="33" max="33"/>
+    <col width="33.1171875" bestFit="1" customWidth="1" style="5" min="34" max="34"/>
+    <col width="56.5859375" bestFit="1" customWidth="1" style="5" min="35" max="35"/>
+    <col width="33.1171875" bestFit="1" customWidth="1" style="5" min="36" max="36"/>
     <col width="30" bestFit="1" customWidth="1" style="5" min="37" max="37"/>
-    <col width="44.7109375" bestFit="1" customWidth="1" style="5" min="38" max="38"/>
-    <col width="39.85546875" bestFit="1" customWidth="1" style="5" min="39" max="39"/>
-    <col width="33.5703125" bestFit="1" customWidth="1" style="5" min="40" max="40"/>
-    <col width="72.28515625" bestFit="1" customWidth="1" style="5" min="41" max="41"/>
+    <col width="44.703125" bestFit="1" customWidth="1" style="5" min="38" max="38"/>
+    <col width="39.87890625" bestFit="1" customWidth="1" style="5" min="39" max="39"/>
+    <col width="33.5859375" bestFit="1" customWidth="1" style="5" min="40" max="40"/>
+    <col width="72.29296875" bestFit="1" customWidth="1" style="5" min="41" max="41"/>
     <col width="52" bestFit="1" customWidth="1" style="5" min="42" max="42"/>
-    <col width="34.42578125" bestFit="1" customWidth="1" style="5" min="43" max="44"/>
-    <col width="47.42578125" bestFit="1" customWidth="1" style="5" min="45" max="46"/>
-    <col width="9.140625" customWidth="1" style="5" min="47" max="16384"/>
+    <col width="34.41015625" bestFit="1" customWidth="1" style="5" min="43" max="44"/>
+    <col width="47.41015625" bestFit="1" customWidth="1" style="5" min="45" max="46"/>
+    <col width="9.1171875" customWidth="1" style="5" min="47" max="16384"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1" s="1">
@@ -1256,8 +1260,8 @@
         </is>
       </c>
     </row>
-    <row r="2" ht="409.5" customFormat="1" customHeight="1" s="2">
-      <c r="A2" s="9" t="inlineStr">
+    <row r="2" ht="409.6" customFormat="1" customHeight="1" s="2">
+      <c r="A2" s="8" t="inlineStr">
         <is>
           <r>
             <rPr>
@@ -1277,11 +1281,12 @@
               <scheme val="minor"/>
             </rPr>
             <t xml:space="preserve">EDFCS-SRO646
+EDFCS-SRO658
 </t>
           </r>
         </is>
       </c>
-      <c r="B2" s="8" t="inlineStr">
+      <c r="B2" s="3" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">EDFCS-SRO465
@@ -1304,7 +1309,7 @@
         </is>
       </c>
       <c r="C2" s="6" t="n"/>
-      <c r="D2" s="8" t="inlineStr">
+      <c r="D2" s="3" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">The EDFCS Autopilot Stabilizer Trim Function shall have increased responsiveness in each of the following conditions except during Fail Op, dual channel approach:
@@ -1362,7 +1367,7 @@
           </r>
         </is>
       </c>
-      <c r="F2" s="8" t="inlineStr">
+      <c r="F2" s="3" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">EDFCS-SRO465
@@ -1527,7 +1532,7 @@
           <t>Inspection</t>
         </is>
       </c>
-      <c r="AH2" s="8" t="inlineStr">
+      <c r="AH2" s="3" t="inlineStr">
         <is>
           <r>
             <t xml:space="preserve">(Inspection) A Requirements Review Board was held on 8/4/2023. Meeting minutes and actions are recorded in EDFCS_SRO465.
@@ -1582,5 +1587,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait"/>
 </worksheet>
 </file>
</xml_diff>